<commit_message>
Added known parts for output and control unit
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Electronics\Projects\8-bit-Breadboard-Computer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\Projects\In progress\8-bit-Breadboard-Computer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
   <si>
     <t>Part</t>
   </si>
@@ -243,6 +243,27 @@
   </si>
   <si>
     <t>http://www.ti.com/lit/ds/symlink/sn74ls86a.pdf</t>
+  </si>
+  <si>
+    <t>EEPROM programmer</t>
+  </si>
+  <si>
+    <t>Required to program the EEPROM chips</t>
+  </si>
+  <si>
+    <t>http://www.alldatasheet.com/datasheet-pdf/pdf/57374/CATALYST/CAT28C16AP-20T.html</t>
+  </si>
+  <si>
+    <t>CAT28C16AP</t>
+  </si>
+  <si>
+    <t>16 Kbit CMOS parellel EEPROM</t>
+  </si>
+  <si>
+    <t>Output, Control Unit</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/191816776888</t>
   </si>
 </sst>
 </file>
@@ -585,22 +606,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E29"/>
+      <selection activeCell="A19" sqref="A19:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.265625" customWidth="1"/>
-    <col min="2" max="2" width="10.59765625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="35.73046875" customWidth="1"/>
-    <col min="4" max="4" width="32.86328125" customWidth="1"/>
-    <col min="5" max="5" width="65.46484375" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" customWidth="1"/>
+    <col min="5" max="5" width="81.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,7 +638,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -631,7 +652,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -645,7 +666,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -662,7 +683,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -679,7 +700,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -696,7 +717,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -713,7 +734,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -730,7 +751,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -747,7 +768,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -764,7 +785,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -781,7 +802,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -798,7 +819,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -815,7 +836,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -832,7 +853,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -846,7 +867,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -857,7 +878,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -868,7 +889,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -879,140 +900,174 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="3">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>36</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B22" s="3">
         <v>5</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B23" s="3">
         <v>5</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B24" s="3">
         <v>33</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B25" s="3">
         <v>11</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B26" s="3">
         <v>1</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>29</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B27" s="3">
         <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="3">
-        <v>8</v>
-      </c>
-      <c r="D26" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="3">
-        <v>2</v>
       </c>
       <c r="D27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B28" s="3">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B29" s="3">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="D29" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="3">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D44">
-    <sortState ref="A2:D43">
-      <sortCondition ref="A1:A43"/>
+  <autoFilter ref="A1:E1">
+    <sortState ref="A2:E31">
+      <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:D42">

</xml_diff>

<commit_message>
Added components for Arduino EEPROM programmer.
Added components for display module (removed 2 obsolete EEPROM chips)
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\Projects\In progress\8-bit-Breadboard-Computer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\BreadboardComputer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14388"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="96">
   <si>
     <t>Part</t>
   </si>
@@ -264,6 +264,57 @@
   </si>
   <si>
     <t>http://www.ebay.com/itm/191816776888</t>
+  </si>
+  <si>
+    <t>Arduino Nano</t>
+  </si>
+  <si>
+    <t>Microcontroller</t>
+  </si>
+  <si>
+    <t>Clock, Output</t>
+  </si>
+  <si>
+    <t>https://www.arduino.cc/en/uploads/Main/ArduinoNanoManual23.pdf</t>
+  </si>
+  <si>
+    <t>74HC595</t>
+  </si>
+  <si>
+    <t>8-bit serial-in, parallel-out shift register</t>
+  </si>
+  <si>
+    <t>http://www.nxp.com/documents/data_sheet/74HC_HCT595.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74LS76 </t>
+  </si>
+  <si>
+    <t>Dual JK flip-flop</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/sn5476.pdf</t>
+  </si>
+  <si>
+    <t>74LS139</t>
+  </si>
+  <si>
+    <t>Dual 2-to-4 line decoder</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/sn54ls139a.pdf</t>
+  </si>
+  <si>
+    <t>7-segment display</t>
+  </si>
+  <si>
+    <t>Common cathode 7-segment display</t>
+  </si>
+  <si>
+    <t>Clock, RAM, Output</t>
   </si>
 </sst>
 </file>
@@ -606,22 +657,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:E20"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" customWidth="1"/>
-    <col min="5" max="5" width="81.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="38.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.88671875" customWidth="1"/>
+    <col min="5" max="5" width="81.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -638,7 +689,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -652,415 +703,497 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>51</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>43</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>42</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B7" s="3">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="3">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
       </c>
       <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="3">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>53</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" t="s">
         <v>54</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B11" s="3">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" t="s">
         <v>44</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>46</v>
-      </c>
-      <c r="B10" s="3">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="3">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>37</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B13" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B14" s="3">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
         <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="B15" s="3">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="B16" s="3">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="E16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B17" s="3">
         <v>2</v>
       </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
       <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="3">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="3">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="3">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B23" s="3">
         <v>2</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B24" s="3">
         <v>6</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C24" t="s">
         <v>76</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D24" t="s">
         <v>77</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B25" s="3">
         <v>1</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C25" t="s">
         <v>73</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D25" t="s">
         <v>77</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E25" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C26" t="s">
         <v>36</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B27" s="3">
         <v>5</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D27" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B28" s="3">
         <v>5</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B29" s="3">
         <v>33</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D29" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B30" s="3">
         <v>11</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>30</v>
-      </c>
-      <c r="B26" s="3">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="3">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="3">
-        <v>8</v>
-      </c>
-      <c r="D28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="3">
-        <v>2</v>
-      </c>
-      <c r="D29" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="3">
-        <v>3</v>
-      </c>
-      <c r="D30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>27</v>
       </c>
       <c r="B31" s="3">
         <v>1</v>
       </c>
       <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="3">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="3">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="3">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" s="3">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
         <v>28</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D36" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated number of EEPROM and added DIP switches
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\BreadboardComputer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Electronics\8-bit-Breadboard-Computer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14388"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14385"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="Re-arrangement (in progress)" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Overview!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Re-arrangement (in progress)'!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="102">
   <si>
     <t>Part</t>
   </si>
@@ -315,13 +317,31 @@
   </si>
   <si>
     <t>Clock, RAM, Output</t>
+  </si>
+  <si>
+    <t>A Register</t>
+  </si>
+  <si>
+    <t>B Register</t>
+  </si>
+  <si>
+    <t>Instruction Register</t>
+  </si>
+  <si>
+    <t>Output Register</t>
+  </si>
+  <si>
+    <t>DIP switch (4 bit)</t>
+  </si>
+  <si>
+    <t>DIP switch (8 bit)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,6 +353,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -367,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -377,6 +404,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,22 +699,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A25" sqref="A25:D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="38.109375" customWidth="1"/>
-    <col min="4" max="4" width="32.88671875" customWidth="1"/>
-    <col min="5" max="5" width="81.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.53125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="38.1328125" customWidth="1"/>
+    <col min="4" max="4" width="32.86328125" customWidth="1"/>
+    <col min="5" max="5" width="81.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -689,7 +731,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -703,7 +745,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -717,7 +759,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -734,7 +776,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -751,7 +793,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -768,7 +810,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -785,7 +827,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -802,7 +844,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -819,7 +861,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -836,7 +878,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -853,7 +895,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -870,7 +912,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -887,7 +929,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -904,7 +946,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -921,7 +963,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -938,7 +980,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -955,7 +997,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>93</v>
       </c>
@@ -969,7 +1011,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -986,7 +1028,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1000,7 +1042,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1011,7 +1053,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1022,7 +1064,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1033,12 +1075,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>75</v>
       </c>
       <c r="B24" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
         <v>76</v>
@@ -1050,156 +1092,178 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="3">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
         <v>73</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D27" t="s">
         <v>77</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E27" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C28" t="s">
         <v>36</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B29" s="3">
         <v>5</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B30" s="3">
         <v>5</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D30" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B31" s="3">
         <v>33</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B32" s="3">
         <v>11</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
         <v>29</v>
       </c>
-      <c r="D31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
         <v>21</v>
-      </c>
-      <c r="B32" s="3">
-        <v>2</v>
-      </c>
-      <c r="D32" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="3">
-        <v>9</v>
-      </c>
-      <c r="D33" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>16</v>
       </c>
       <c r="B34" s="3">
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="3">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="3">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B37" s="3">
         <v>3</v>
       </c>
-      <c r="D35" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="3">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
         <v>28</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D38" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1">
-    <sortState ref="A2:E31">
+    <sortState ref="A2:E38">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
@@ -1209,4 +1273,931 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E70"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.53125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="38.1328125" customWidth="1"/>
+    <col min="4" max="4" width="32.86328125" customWidth="1"/>
+    <col min="5" max="5" width="81.46484375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="6">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="11">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3">
+        <v>3</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6">
+        <v>3</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="10">
+        <v>2</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="6">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="6">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="3">
+        <v>16</v>
+      </c>
+      <c r="C37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="3">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="3">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="3">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="3">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="3">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="3">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="3">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="3">
+        <v>5</v>
+      </c>
+      <c r="D49" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" s="3">
+        <v>11</v>
+      </c>
+      <c r="D50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" s="3">
+        <v>4</v>
+      </c>
+      <c r="D51" t="s">
+        <v>81</v>
+      </c>
+      <c r="E51" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="3">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="3">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" s="3">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" s="3">
+        <v>9</v>
+      </c>
+      <c r="D55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" s="3">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" t="s">
+        <v>72</v>
+      </c>
+      <c r="E56" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>79</v>
+      </c>
+      <c r="B57" s="3">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>80</v>
+      </c>
+      <c r="D57" t="s">
+        <v>72</v>
+      </c>
+      <c r="E57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58" s="3">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>91</v>
+      </c>
+      <c r="D58" t="s">
+        <v>88</v>
+      </c>
+      <c r="E58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>86</v>
+      </c>
+      <c r="B59" s="3">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>87</v>
+      </c>
+      <c r="D59" t="s">
+        <v>88</v>
+      </c>
+      <c r="E59" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>93</v>
+      </c>
+      <c r="B60" s="3">
+        <v>4</v>
+      </c>
+      <c r="C60" t="s">
+        <v>94</v>
+      </c>
+      <c r="D60" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" s="3">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" t="s">
+        <v>77</v>
+      </c>
+      <c r="E61" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>72</v>
+      </c>
+      <c r="B62" s="3">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62" t="s">
+        <v>77</v>
+      </c>
+      <c r="E62" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>52</v>
+      </c>
+      <c r="B63" s="3">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>53</v>
+      </c>
+      <c r="D63" t="s">
+        <v>54</v>
+      </c>
+      <c r="E63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>50</v>
+      </c>
+      <c r="B64" s="3">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>51</v>
+      </c>
+      <c r="D64" t="s">
+        <v>43</v>
+      </c>
+      <c r="E64" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>48</v>
+      </c>
+      <c r="B65" s="3">
+        <v>4</v>
+      </c>
+      <c r="C65" t="s">
+        <v>49</v>
+      </c>
+      <c r="D65" t="s">
+        <v>43</v>
+      </c>
+      <c r="E65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>46</v>
+      </c>
+      <c r="B66" s="3">
+        <v>2</v>
+      </c>
+      <c r="C66" t="s">
+        <v>47</v>
+      </c>
+      <c r="D66" t="s">
+        <v>43</v>
+      </c>
+      <c r="E66" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67" s="3">
+        <v>5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>33</v>
+      </c>
+      <c r="B68" s="3">
+        <v>6</v>
+      </c>
+      <c r="C68" t="s">
+        <v>34</v>
+      </c>
+      <c r="D68" t="s">
+        <v>55</v>
+      </c>
+      <c r="E68" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69" s="3">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s">
+        <v>32</v>
+      </c>
+      <c r="D69" t="s">
+        <v>44</v>
+      </c>
+      <c r="E69" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" s="3">
+        <v>33</v>
+      </c>
+      <c r="D70" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E1">
+    <sortState ref="A2:E65">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
+  <sortState ref="A37:E70">
+    <sortCondition ref="D37:D70"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated layout for parts list
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -526,21 +526,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -564,10 +549,25 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -851,6 +851,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -867,80 +870,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="29" t="s">
+      <c r="B3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="18">
         <v>16</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="24"/>
+      <c r="D5" s="19"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="26">
-        <v>1</v>
-      </c>
-      <c r="C6" s="25" t="s">
+      <c r="B6" s="21">
+        <v>1</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="20" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
     </row>
     <row r="8" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="10"/>
@@ -950,186 +953,186 @@
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="29" t="s">
+      <c r="B11" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="18">
         <v>3</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="20" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="23">
-        <v>1</v>
-      </c>
-      <c r="C13" s="25" t="s">
+      <c r="B13" s="18">
+        <v>1</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="20" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="26">
-        <v>1</v>
-      </c>
-      <c r="C14" s="25" t="s">
+      <c r="B14" s="21">
+        <v>1</v>
+      </c>
+      <c r="C14" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="26">
-        <v>1</v>
-      </c>
-      <c r="C15" s="25" t="s">
+      <c r="B15" s="21">
+        <v>1</v>
+      </c>
+      <c r="C15" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="20" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="18">
         <v>3</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="27">
-        <v>2</v>
-      </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
+      <c r="B17" s="22">
+        <v>2</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="26">
-        <v>1</v>
-      </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
+      <c r="B18" s="21">
+        <v>1</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="23">
-        <v>1</v>
-      </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
+      <c r="B19" s="18">
+        <v>1</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="26">
-        <v>1</v>
-      </c>
-      <c r="C20" s="25" t="s">
+      <c r="B20" s="21">
+        <v>1</v>
+      </c>
+      <c r="C20" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="24"/>
+      <c r="D20" s="19"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="23">
+      <c r="B21" s="18">
         <v>5</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="26">
-        <v>1</v>
-      </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
+      <c r="B22" s="21">
+        <v>1</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="26">
-        <v>1</v>
-      </c>
-      <c r="C23" s="25" t="s">
+      <c r="B23" s="21">
+        <v>1</v>
+      </c>
+      <c r="C23" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="24"/>
+      <c r="D23" s="19"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B24" s="26">
-        <v>1</v>
-      </c>
-      <c r="C24" s="24" t="s">
+      <c r="B24" s="21">
+        <v>1</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="24"/>
+      <c r="D24" s="19"/>
     </row>
     <row r="25" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="10"/>
@@ -1138,73 +1141,73 @@
       <c r="D25" s="13"/>
     </row>
     <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
     </row>
     <row r="27" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="29" t="s">
+      <c r="B28" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="24" t="s">
         <v>46</v>
       </c>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="26">
-        <v>2</v>
-      </c>
-      <c r="C29" s="25" t="s">
+      <c r="B29" s="21">
+        <v>2</v>
+      </c>
+      <c r="C29" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="20" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="26">
-        <v>1</v>
-      </c>
-      <c r="C30" s="25" t="s">
+      <c r="B30" s="21">
+        <v>1</v>
+      </c>
+      <c r="C30" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="20" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="26">
+      <c r="B31" s="21">
         <v>8</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
     </row>
     <row r="32" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="14"/>
@@ -1214,77 +1217,77 @@
       <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
       <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
       <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" s="29" t="s">
+      <c r="B35" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="24" t="s">
         <v>46</v>
       </c>
       <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="26">
-        <v>2</v>
-      </c>
-      <c r="C36" s="25" t="s">
+      <c r="B36" s="21">
+        <v>2</v>
+      </c>
+      <c r="C36" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="25" t="s">
+      <c r="D36" s="20" t="s">
         <v>53</v>
       </c>
       <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="26">
-        <v>1</v>
-      </c>
-      <c r="C37" s="25" t="s">
+      <c r="B37" s="21">
+        <v>1</v>
+      </c>
+      <c r="C37" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D37" s="25" t="s">
+      <c r="D37" s="20" t="s">
         <v>55</v>
       </c>
       <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="26">
+      <c r="B38" s="21">
         <v>8</v>
       </c>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
       <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1295,88 +1298,88 @@
       <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
       <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
       <c r="E41" s="4"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42" s="29" t="s">
+      <c r="B42" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="24" t="s">
         <v>46</v>
       </c>
       <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B43" s="26">
-        <v>2</v>
-      </c>
-      <c r="C43" s="25" t="s">
+      <c r="B43" s="21">
+        <v>2</v>
+      </c>
+      <c r="C43" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D43" s="25" t="s">
+      <c r="D43" s="20" t="s">
         <v>53</v>
       </c>
       <c r="E43" s="4"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="26">
-        <v>1</v>
-      </c>
-      <c r="C44" s="25" t="s">
+      <c r="B44" s="21">
+        <v>1</v>
+      </c>
+      <c r="C44" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D44" s="25" t="s">
+      <c r="D44" s="20" t="s">
         <v>55</v>
       </c>
       <c r="E44" s="4"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="26">
+      <c r="B45" s="21">
         <v>4</v>
       </c>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
       <c r="E45" s="4"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A46" s="25" t="s">
+      <c r="A46" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="26">
+      <c r="B46" s="21">
         <v>4</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
       <c r="E46" s="4"/>
     </row>
     <row r="47" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1387,358 +1390,358 @@
       <c r="E47" s="4"/>
     </row>
     <row r="48" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="19"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
       <c r="E48" s="4"/>
     </row>
     <row r="49" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
       <c r="E49" s="4"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D50" s="29" t="s">
+      <c r="B50" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="24" t="s">
         <v>46</v>
       </c>
       <c r="E50" s="4"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A51" s="25" t="s">
+      <c r="A51" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B51" s="26">
-        <v>1</v>
-      </c>
-      <c r="C51" s="25" t="s">
+      <c r="B51" s="21">
+        <v>1</v>
+      </c>
+      <c r="C51" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D51" s="25" t="s">
+      <c r="D51" s="20" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A52" s="25" t="s">
+      <c r="A52" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B52" s="26">
-        <v>2</v>
-      </c>
-      <c r="C52" s="25" t="s">
+      <c r="B52" s="21">
+        <v>2</v>
+      </c>
+      <c r="C52" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D52" s="25" t="s">
+      <c r="D52" s="20" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A53" s="25" t="s">
+      <c r="A53" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B53" s="26">
-        <v>2</v>
-      </c>
-      <c r="C53" s="25" t="s">
+      <c r="B53" s="21">
+        <v>2</v>
+      </c>
+      <c r="C53" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="25" t="s">
+      <c r="D53" s="20" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A54" s="25" t="s">
+      <c r="A54" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B54" s="26">
+      <c r="B54" s="21">
         <v>8</v>
       </c>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
       <c r="E54" s="4"/>
     </row>
     <row r="55" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E55" s="4"/>
     </row>
     <row r="56" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A56" s="19" t="s">
+      <c r="A56" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="B56" s="19"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
       <c r="E56" s="4"/>
     </row>
     <row r="57" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="31" t="s">
+      <c r="A57" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="B57" s="32"/>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
       <c r="E57" s="4"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A58" s="29" t="s">
+      <c r="A58" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B58" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D58" s="29" t="s">
+      <c r="B58" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="24" t="s">
         <v>46</v>
       </c>
       <c r="E58" s="4"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A59" s="25" t="s">
+      <c r="A59" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B59" s="26">
-        <v>1</v>
-      </c>
-      <c r="C59" s="25" t="s">
+      <c r="B59" s="21">
+        <v>1</v>
+      </c>
+      <c r="C59" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D59" s="25" t="s">
+      <c r="D59" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A60" s="25" t="s">
+      <c r="A60" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B60" s="26">
-        <v>2</v>
-      </c>
-      <c r="C60" s="25" t="s">
+      <c r="B60" s="21">
+        <v>2</v>
+      </c>
+      <c r="C60" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D60" s="25" t="s">
+      <c r="D60" s="20" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A61" s="25" t="s">
+      <c r="A61" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B61" s="26">
+      <c r="B61" s="21">
         <v>4</v>
       </c>
-      <c r="C61" s="25" t="s">
+      <c r="C61" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D61" s="25" t="s">
+      <c r="D61" s="20" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A62" s="25" t="s">
+      <c r="A62" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B62" s="26">
-        <v>1</v>
-      </c>
-      <c r="C62" s="25" t="s">
+      <c r="B62" s="21">
+        <v>1</v>
+      </c>
+      <c r="C62" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D62" s="25" t="s">
+      <c r="D62" s="20" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A63" s="25" t="s">
+      <c r="A63" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B63" s="26">
-        <v>2</v>
-      </c>
-      <c r="C63" s="25" t="s">
+      <c r="B63" s="21">
+        <v>2</v>
+      </c>
+      <c r="C63" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D63" s="25" t="s">
+      <c r="D63" s="20" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A64" s="25" t="s">
+      <c r="A64" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B64" s="26">
-        <v>1</v>
-      </c>
-      <c r="C64" s="25" t="s">
+      <c r="B64" s="21">
+        <v>1</v>
+      </c>
+      <c r="C64" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D64" s="25" t="s">
+      <c r="D64" s="20" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A65" s="25" t="s">
+      <c r="A65" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B65" s="26">
-        <v>1</v>
-      </c>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
+      <c r="B65" s="21">
+        <v>1</v>
+      </c>
+      <c r="C65" s="20"/>
+      <c r="D65" s="20"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A66" s="25" t="s">
+      <c r="A66" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B66" s="26">
-        <v>1</v>
-      </c>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
+      <c r="B66" s="21">
+        <v>1</v>
+      </c>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A67" s="25" t="s">
+      <c r="A67" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B67" s="26">
-        <v>1</v>
-      </c>
-      <c r="C67" s="25"/>
-      <c r="D67" s="25"/>
+      <c r="B67" s="21">
+        <v>1</v>
+      </c>
+      <c r="C67" s="20"/>
+      <c r="D67" s="20"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A68" s="25" t="s">
+      <c r="A68" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B68" s="26">
+      <c r="B68" s="21">
         <v>9</v>
       </c>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="20"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A69" s="25" t="s">
+      <c r="A69" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B69" s="26">
+      <c r="B69" s="21">
         <v>4</v>
       </c>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A70" s="25" t="s">
+      <c r="A70" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B70" s="26">
-        <v>1</v>
-      </c>
-      <c r="C70" s="25" t="s">
+      <c r="B70" s="21">
+        <v>1</v>
+      </c>
+      <c r="C70" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D70" s="25"/>
+      <c r="D70" s="20"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A71" s="25" t="s">
+      <c r="A71" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B71" s="26">
-        <v>2</v>
-      </c>
-      <c r="C71" s="25"/>
-      <c r="D71" s="25"/>
+      <c r="B71" s="21">
+        <v>2</v>
+      </c>
+      <c r="C71" s="20"/>
+      <c r="D71" s="20"/>
       <c r="E71" s="4"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A72" s="25" t="s">
+      <c r="A72" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B72" s="26">
-        <v>1</v>
-      </c>
-      <c r="C72" s="25" t="s">
+      <c r="B72" s="21">
+        <v>1</v>
+      </c>
+      <c r="C72" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D72" s="25"/>
+      <c r="D72" s="20"/>
       <c r="E72" s="4"/>
     </row>
     <row r="73" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E73" s="4"/>
     </row>
     <row r="74" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A74" s="19" t="s">
+      <c r="A74" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="B74" s="19"/>
-      <c r="C74" s="19"/>
-      <c r="D74" s="19"/>
+      <c r="B74" s="28"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
       <c r="E74" s="4"/>
     </row>
     <row r="75" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" s="31" t="s">
+      <c r="A75" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="B75" s="32"/>
-      <c r="C75" s="32"/>
-      <c r="D75" s="32"/>
+      <c r="B75" s="27"/>
+      <c r="C75" s="27"/>
+      <c r="D75" s="27"/>
       <c r="E75" s="4"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A76" s="29" t="s">
+      <c r="A76" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B76" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C76" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D76" s="29" t="s">
+      <c r="B76" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" s="24" t="s">
         <v>46</v>
       </c>
       <c r="E76" s="4"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A77" s="25" t="s">
+      <c r="A77" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B77" s="26">
-        <v>2</v>
-      </c>
-      <c r="C77" s="25" t="s">
+      <c r="B77" s="21">
+        <v>2</v>
+      </c>
+      <c r="C77" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D77" s="25" t="s">
+      <c r="D77" s="20" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A78" s="25" t="s">
+      <c r="A78" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B78" s="26">
-        <v>1</v>
-      </c>
-      <c r="C78" s="25" t="s">
+      <c r="B78" s="21">
+        <v>1</v>
+      </c>
+      <c r="C78" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D78" s="25" t="s">
+      <c r="D78" s="20" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1750,268 +1753,268 @@
       <c r="E79" s="4"/>
     </row>
     <row r="80" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A80" s="19" t="s">
+      <c r="A80" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B80" s="19"/>
-      <c r="C80" s="19"/>
-      <c r="D80" s="19"/>
+      <c r="B80" s="28"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="28"/>
       <c r="E80" s="4"/>
     </row>
     <row r="81" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A81" s="31" t="s">
+      <c r="A81" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="B81" s="32"/>
-      <c r="C81" s="32"/>
-      <c r="D81" s="32"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
       <c r="E81" s="4"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A82" s="29" t="s">
+      <c r="A82" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B82" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C82" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D82" s="29" t="s">
+      <c r="B82" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82" s="24" t="s">
         <v>46</v>
       </c>
       <c r="E82" s="4"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A83" s="25" t="s">
+      <c r="A83" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B83" s="26">
-        <v>1</v>
-      </c>
-      <c r="C83" s="25"/>
-      <c r="D83" s="25" t="s">
+      <c r="B83" s="21">
+        <v>1</v>
+      </c>
+      <c r="C83" s="20"/>
+      <c r="D83" s="20" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A84" s="25" t="s">
+      <c r="A84" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B84" s="26">
-        <v>1</v>
-      </c>
-      <c r="C84" s="25" t="s">
+      <c r="B84" s="21">
+        <v>1</v>
+      </c>
+      <c r="C84" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D84" s="25" t="s">
+      <c r="D84" s="20" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A85" s="25" t="s">
+      <c r="A85" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B85" s="26">
-        <v>1</v>
-      </c>
-      <c r="C85" s="25" t="s">
+      <c r="B85" s="21">
+        <v>1</v>
+      </c>
+      <c r="C85" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D85" s="25" t="s">
+      <c r="D85" s="20" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A86" s="25" t="s">
+      <c r="A86" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="B86" s="26">
+      <c r="B86" s="21">
         <v>4</v>
       </c>
-      <c r="C86" s="25" t="s">
+      <c r="C86" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D86" s="25"/>
+      <c r="D86" s="20"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A87" s="25" t="s">
+      <c r="A87" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B87" s="26">
-        <v>2</v>
-      </c>
-      <c r="C87" s="25"/>
-      <c r="D87" s="25"/>
+      <c r="B87" s="21">
+        <v>2</v>
+      </c>
+      <c r="C87" s="20"/>
+      <c r="D87" s="20"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A88" s="25" t="s">
+      <c r="A88" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B88" s="26">
-        <v>1</v>
-      </c>
-      <c r="C88" s="25" t="s">
+      <c r="B88" s="21">
+        <v>1</v>
+      </c>
+      <c r="C88" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="D88" s="25" t="s">
+      <c r="D88" s="20" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A89" s="25" t="s">
+      <c r="A89" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B89" s="26">
-        <v>1</v>
-      </c>
-      <c r="C89" s="25"/>
-      <c r="D89" s="25"/>
+      <c r="B89" s="21">
+        <v>1</v>
+      </c>
+      <c r="C89" s="20"/>
+      <c r="D89" s="20"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A90" s="25" t="s">
+      <c r="A90" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B90" s="26">
-        <v>1</v>
-      </c>
-      <c r="C90" s="25"/>
-      <c r="D90" s="25"/>
+      <c r="B90" s="21">
+        <v>1</v>
+      </c>
+      <c r="C90" s="20"/>
+      <c r="D90" s="20"/>
     </row>
     <row r="91" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="92" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A92" s="19" t="s">
+      <c r="A92" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="B92" s="19"/>
-      <c r="C92" s="19"/>
-      <c r="D92" s="19"/>
+      <c r="B92" s="28"/>
+      <c r="C92" s="28"/>
+      <c r="D92" s="28"/>
     </row>
     <row r="93" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" s="31" t="s">
+      <c r="A93" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B93" s="32"/>
-      <c r="C93" s="32"/>
-      <c r="D93" s="32"/>
+      <c r="B93" s="27"/>
+      <c r="C93" s="27"/>
+      <c r="D93" s="27"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A94" s="29" t="s">
+      <c r="A94" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B94" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C94" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D94" s="29" t="s">
+      <c r="B94" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D94" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A95" s="25" t="s">
+      <c r="A95" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B95" s="26">
-        <v>1</v>
-      </c>
-      <c r="C95" s="25" t="s">
+      <c r="B95" s="21">
+        <v>1</v>
+      </c>
+      <c r="C95" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D95" s="25" t="s">
+      <c r="D95" s="20" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A96" s="25" t="s">
+      <c r="A96" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B96" s="26">
-        <v>1</v>
-      </c>
-      <c r="C96" s="25" t="s">
+      <c r="B96" s="21">
+        <v>1</v>
+      </c>
+      <c r="C96" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D96" s="25" t="s">
+      <c r="D96" s="20" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A97" s="25" t="s">
+      <c r="A97" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B97" s="26">
+      <c r="B97" s="21">
         <v>4</v>
       </c>
-      <c r="C97" s="25"/>
-      <c r="D97" s="25"/>
+      <c r="C97" s="20"/>
+      <c r="D97" s="20"/>
     </row>
     <row r="98" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="99" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A99" s="19" t="s">
+      <c r="A99" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="B99" s="19"/>
-      <c r="C99" s="19"/>
-      <c r="D99" s="19"/>
+      <c r="B99" s="28"/>
+      <c r="C99" s="28"/>
+      <c r="D99" s="28"/>
     </row>
     <row r="100" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A100" s="33" t="s">
+      <c r="A100" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="B100" s="34"/>
-      <c r="C100" s="34"/>
-      <c r="D100" s="34"/>
+      <c r="B100" s="30"/>
+      <c r="C100" s="30"/>
+      <c r="D100" s="30"/>
     </row>
     <row r="101" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="21" t="s">
+      <c r="A101" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="B101" s="21"/>
-      <c r="C101" s="21"/>
-      <c r="D101" s="21"/>
+      <c r="B101" s="31"/>
+      <c r="C101" s="31"/>
+      <c r="D101" s="31"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A102" s="29" t="s">
+      <c r="A102" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B102" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C102" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D102" s="29" t="s">
+      <c r="B102" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D102" s="24" t="s">
         <v>46</v>
       </c>
       <c r="E102" s="4"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A103" s="25" t="s">
+      <c r="A103" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B103" s="26">
-        <v>1</v>
-      </c>
-      <c r="C103" s="25" t="s">
+      <c r="B103" s="21">
+        <v>1</v>
+      </c>
+      <c r="C103" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D103" s="25" t="s">
+      <c r="D103" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A104" s="25" t="s">
+      <c r="A104" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="B104" s="26">
-        <v>1</v>
-      </c>
-      <c r="C104" s="25" t="s">
+      <c r="B104" s="21">
+        <v>1</v>
+      </c>
+      <c r="C104" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="D104" s="25" t="s">
+      <c r="D104" s="20" t="s">
         <v>104</v>
       </c>
       <c r="E104" s="4"/>
@@ -2020,137 +2023,137 @@
       <c r="E105" s="4"/>
     </row>
     <row r="106" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A106" s="19" t="s">
+      <c r="A106" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="B106" s="19"/>
-      <c r="C106" s="19"/>
-      <c r="D106" s="19"/>
+      <c r="B106" s="28"/>
+      <c r="C106" s="28"/>
+      <c r="D106" s="28"/>
       <c r="E106" s="4"/>
     </row>
     <row r="107" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" s="31" t="s">
+      <c r="A107" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B107" s="32"/>
-      <c r="C107" s="32"/>
-      <c r="D107" s="32"/>
+      <c r="B107" s="27"/>
+      <c r="C107" s="27"/>
+      <c r="D107" s="27"/>
       <c r="E107" s="4"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A108" s="29" t="s">
+      <c r="A108" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B108" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C108" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D108" s="29" t="s">
+      <c r="B108" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D108" s="24" t="s">
         <v>46</v>
       </c>
       <c r="E108" s="4"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A109" s="25" t="s">
+      <c r="A109" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B109" s="26">
+      <c r="B109" s="21">
         <v>8</v>
       </c>
-      <c r="C109" s="24" t="s">
+      <c r="C109" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D109" s="25"/>
+      <c r="D109" s="20"/>
       <c r="E109" s="4"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A110" s="25" t="s">
+      <c r="A110" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B110" s="26">
+      <c r="B110" s="21">
         <v>8</v>
       </c>
-      <c r="C110" s="25"/>
-      <c r="D110" s="25"/>
+      <c r="C110" s="20"/>
+      <c r="D110" s="20"/>
       <c r="E110" s="4"/>
     </row>
     <row r="111" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E111" s="4"/>
     </row>
     <row r="112" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A112" s="19" t="s">
+      <c r="A112" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="B112" s="19"/>
-      <c r="C112" s="19"/>
-      <c r="D112" s="19"/>
+      <c r="B112" s="28"/>
+      <c r="C112" s="28"/>
+      <c r="D112" s="28"/>
       <c r="E112" s="4"/>
     </row>
     <row r="113" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A113" s="31" t="s">
+      <c r="A113" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B113" s="32"/>
-      <c r="C113" s="32"/>
-      <c r="D113" s="32"/>
+      <c r="B113" s="27"/>
+      <c r="C113" s="27"/>
+      <c r="D113" s="27"/>
       <c r="E113" s="4"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A114" s="29" t="s">
+      <c r="A114" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B114" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C114" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D114" s="29" t="s">
+      <c r="B114" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C114" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D114" s="24" t="s">
         <v>46</v>
       </c>
       <c r="E114" s="4"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A115" s="25" t="s">
+      <c r="A115" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B115" s="26">
-        <v>1</v>
-      </c>
-      <c r="C115" s="25" t="s">
+      <c r="B115" s="21">
+        <v>1</v>
+      </c>
+      <c r="C115" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D115" s="25" t="s">
+      <c r="D115" s="20" t="s">
         <v>52</v>
       </c>
       <c r="E115" s="4"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A116" s="25" t="s">
+      <c r="A116" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B116" s="26">
-        <v>1</v>
-      </c>
-      <c r="C116" s="25" t="s">
+      <c r="B116" s="21">
+        <v>1</v>
+      </c>
+      <c r="C116" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D116" s="25" t="s">
+      <c r="D116" s="20" t="s">
         <v>55</v>
       </c>
       <c r="E116" s="4"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A117" s="25" t="s">
+      <c r="A117" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B117" s="26">
+      <c r="B117" s="21">
         <v>4</v>
       </c>
-      <c r="C117" s="25"/>
-      <c r="D117" s="25"/>
+      <c r="C117" s="20"/>
+      <c r="D117" s="20"/>
       <c r="E117" s="4"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.45">
@@ -2185,20 +2188,6 @@
     <sortCondition ref="A95"/>
   </sortState>
   <mergeCells count="27">
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A112:D112"/>
-    <mergeCell ref="A113:D113"/>
-    <mergeCell ref="A100:D100"/>
-    <mergeCell ref="A92:D92"/>
-    <mergeCell ref="A93:D93"/>
-    <mergeCell ref="A99:D99"/>
-    <mergeCell ref="A101:D101"/>
-    <mergeCell ref="A106:D106"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A33:D33"/>
     <mergeCell ref="A81:D81"/>
     <mergeCell ref="A40:D40"/>
     <mergeCell ref="A41:D41"/>
@@ -2212,6 +2201,20 @@
     <mergeCell ref="A74:D74"/>
     <mergeCell ref="A75:D75"/>
     <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A113:D113"/>
+    <mergeCell ref="A100:D100"/>
+    <mergeCell ref="A92:D92"/>
+    <mergeCell ref="A93:D93"/>
+    <mergeCell ref="A99:D99"/>
+    <mergeCell ref="A101:D101"/>
+    <mergeCell ref="A106:D106"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
@@ -2229,6 +2232,6 @@
     <hyperlink ref="A113" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" scale="86" fitToHeight="0" orientation="landscape" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added parts for latest video. Added labels for control line wires
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Electronics\8-bit-Breadboard-Computer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\Projects\In progress\8-bit-Breadboard-Computer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="113">
   <si>
     <t>Part</t>
   </si>
@@ -353,16 +353,28 @@
     <t>Resistor 10kΩ</t>
   </si>
   <si>
-    <t>Control Unit</t>
-  </si>
-  <si>
     <t>This module can also be build in the same way as the A/B/Instruction Register if you don't have the additional 74LS273 which is not used in any other module (so far)</t>
+  </si>
+  <si>
+    <t>Control Word</t>
+  </si>
+  <si>
+    <t>Resistor 470Ω</t>
+  </si>
+  <si>
+    <t>Current limiting resistors for the LEDs</t>
+  </si>
+  <si>
+    <t>Pull down resistors</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=AwUirxi9eBg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -549,7 +561,16 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -559,15 +580,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -854,30 +866,30 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.53125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.1328125" customWidth="1"/>
-    <col min="4" max="4" width="73.9296875" customWidth="1"/>
-    <col min="5" max="5" width="81.46484375" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="4" max="4" width="74" customWidth="1"/>
+    <col min="5" max="5" width="81.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-    </row>
-    <row r="2" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>87</v>
       </c>
@@ -885,7 +897,7 @@
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>0</v>
       </c>
@@ -899,7 +911,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>16</v>
       </c>
@@ -909,7 +921,7 @@
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>44</v>
       </c>
@@ -921,7 +933,7 @@
       </c>
       <c r="D5" s="19"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>94</v>
       </c>
@@ -935,7 +947,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>30</v>
       </c>
@@ -945,23 +957,23 @@
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
     </row>
-    <row r="8" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A9" s="32" t="s">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>86</v>
       </c>
@@ -970,7 +982,7 @@
       <c r="D10" s="27"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>0</v>
       </c>
@@ -984,7 +996,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>13</v>
       </c>
@@ -996,7 +1008,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>3</v>
       </c>
@@ -1010,7 +1022,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>5</v>
       </c>
@@ -1024,7 +1036,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>7</v>
       </c>
@@ -1038,7 +1050,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>20</v>
       </c>
@@ -1048,7 +1060,7 @@
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>19</v>
       </c>
@@ -1058,7 +1070,7 @@
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>18</v>
       </c>
@@ -1068,7 +1080,7 @@
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>11</v>
       </c>
@@ -1078,7 +1090,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>25</v>
       </c>
@@ -1090,7 +1102,7 @@
       </c>
       <c r="D20" s="19"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>14</v>
       </c>
@@ -1100,7 +1112,7 @@
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>15</v>
       </c>
@@ -1110,7 +1122,7 @@
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>22</v>
       </c>
@@ -1122,7 +1134,7 @@
       </c>
       <c r="D23" s="19"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>83</v>
       </c>
@@ -1134,21 +1146,21 @@
       </c>
       <c r="D24" s="19"/>
     </row>
-    <row r="25" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="12"/>
       <c r="D25" s="13"/>
     </row>
-    <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A26" s="28" t="s">
+    <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A26" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-    </row>
-    <row r="27" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+    </row>
+    <row r="27" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="26" t="s">
         <v>85</v>
       </c>
@@ -1156,7 +1168,7 @@
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
@@ -1171,7 +1183,7 @@
       </c>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>26</v>
       </c>
@@ -1185,7 +1197,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
         <v>28</v>
       </c>
@@ -1199,7 +1211,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>9</v>
       </c>
@@ -1209,23 +1221,23 @@
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
     </row>
-    <row r="32" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
       <c r="B32" s="15"/>
       <c r="C32" s="14"/>
       <c r="D32" s="16"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A33" s="34" t="s">
+    <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A33" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="26" t="s">
         <v>85</v>
       </c>
@@ -1234,7 +1246,7 @@
       <c r="D34" s="27"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
         <v>0</v>
       </c>
@@ -1249,7 +1261,7 @@
       </c>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
         <v>26</v>
       </c>
@@ -1264,7 +1276,7 @@
       </c>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>28</v>
       </c>
@@ -1279,7 +1291,7 @@
       </c>
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
         <v>9</v>
       </c>
@@ -1290,23 +1302,23 @@
       <c r="D38" s="20"/>
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14"/>
       <c r="B39" s="15"/>
       <c r="C39" s="14"/>
       <c r="D39" s="16"/>
       <c r="E39" s="4"/>
     </row>
-    <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A40" s="34" t="s">
+    <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A40" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
       <c r="E40" s="4"/>
     </row>
-    <row r="41" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="26" t="s">
         <v>85</v>
       </c>
@@ -1315,7 +1327,7 @@
       <c r="D41" s="27"/>
       <c r="E41" s="4"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>0</v>
       </c>
@@ -1330,7 +1342,7 @@
       </c>
       <c r="E42" s="4"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>26</v>
       </c>
@@ -1345,7 +1357,7 @@
       </c>
       <c r="E43" s="4"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
         <v>28</v>
       </c>
@@ -1360,7 +1372,7 @@
       </c>
       <c r="E44" s="4"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>11</v>
       </c>
@@ -1371,7 +1383,7 @@
       <c r="D45" s="20"/>
       <c r="E45" s="4"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>12</v>
       </c>
@@ -1382,23 +1394,23 @@
       <c r="D46" s="23"/>
       <c r="E46" s="4"/>
     </row>
-    <row r="47" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="14"/>
       <c r="B47" s="15"/>
       <c r="C47" s="14"/>
       <c r="D47" s="16"/>
       <c r="E47" s="4"/>
     </row>
-    <row r="48" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A48" s="28" t="s">
+    <row r="48" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A48" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="28"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
       <c r="E48" s="4"/>
     </row>
-    <row r="49" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="26" t="s">
         <v>88</v>
       </c>
@@ -1407,7 +1419,7 @@
       <c r="D49" s="27"/>
       <c r="E49" s="4"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
         <v>0</v>
       </c>
@@ -1422,7 +1434,7 @@
       </c>
       <c r="E50" s="4"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>28</v>
       </c>
@@ -1436,7 +1448,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>31</v>
       </c>
@@ -1450,7 +1462,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
         <v>34</v>
       </c>
@@ -1464,7 +1476,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>9</v>
       </c>
@@ -1475,19 +1487,19 @@
       <c r="D54" s="20"/>
       <c r="E54" s="4"/>
     </row>
-    <row r="55" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E55" s="4"/>
     </row>
-    <row r="56" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A56" s="28" t="s">
+    <row r="56" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A56" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="B56" s="28"/>
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="29"/>
       <c r="E56" s="4"/>
     </row>
-    <row r="57" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="26" t="s">
         <v>90</v>
       </c>
@@ -1496,7 +1508,7 @@
       <c r="D57" s="27"/>
       <c r="E57" s="4"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="24" t="s">
         <v>0</v>
       </c>
@@ -1511,7 +1523,7 @@
       </c>
       <c r="E58" s="4"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
         <v>40</v>
       </c>
@@ -1525,7 +1537,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
         <v>3</v>
       </c>
@@ -1539,7 +1551,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
         <v>38</v>
       </c>
@@ -1553,7 +1565,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
         <v>26</v>
       </c>
@@ -1567,7 +1579,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
         <v>36</v>
       </c>
@@ -1581,7 +1593,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
         <v>28</v>
       </c>
@@ -1595,7 +1607,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
         <v>79</v>
       </c>
@@ -1605,7 +1617,7 @@
       <c r="C65" s="20"/>
       <c r="D65" s="20"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
         <v>80</v>
       </c>
@@ -1615,7 +1627,7 @@
       <c r="C66" s="20"/>
       <c r="D66" s="20"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
         <v>10</v>
       </c>
@@ -1625,7 +1637,7 @@
       <c r="C67" s="20"/>
       <c r="D67" s="20"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
         <v>9</v>
       </c>
@@ -1635,7 +1647,7 @@
       <c r="C68" s="20"/>
       <c r="D68" s="20"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
         <v>12</v>
       </c>
@@ -1645,7 +1657,7 @@
       <c r="C69" s="20"/>
       <c r="D69" s="20"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
         <v>25</v>
       </c>
@@ -1657,7 +1669,7 @@
       </c>
       <c r="D70" s="20"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="s">
         <v>14</v>
       </c>
@@ -1668,7 +1680,7 @@
       <c r="D71" s="20"/>
       <c r="E71" s="4"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
         <v>22</v>
       </c>
@@ -1681,19 +1693,19 @@
       <c r="D72" s="20"/>
       <c r="E72" s="4"/>
     </row>
-    <row r="73" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E73" s="4"/>
     </row>
-    <row r="74" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A74" s="28" t="s">
+    <row r="74" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A74" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="B74" s="28"/>
-      <c r="C74" s="28"/>
-      <c r="D74" s="28"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="29"/>
       <c r="E74" s="4"/>
     </row>
-    <row r="75" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="26" t="s">
         <v>91</v>
       </c>
@@ -1702,7 +1714,7 @@
       <c r="D75" s="27"/>
       <c r="E75" s="4"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
         <v>0</v>
       </c>
@@ -1717,7 +1729,7 @@
       </c>
       <c r="E76" s="4"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="20" t="s">
         <v>65</v>
       </c>
@@ -1731,7 +1743,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="20" t="s">
         <v>62</v>
       </c>
@@ -1745,23 +1757,23 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="7"/>
       <c r="B79" s="8"/>
       <c r="C79" s="7"/>
       <c r="D79" s="9"/>
       <c r="E79" s="4"/>
     </row>
-    <row r="80" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A80" s="28" t="s">
+    <row r="80" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A80" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="B80" s="28"/>
-      <c r="C80" s="28"/>
-      <c r="D80" s="28"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="29"/>
+      <c r="D80" s="29"/>
       <c r="E80" s="4"/>
     </row>
-    <row r="81" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="26" t="s">
         <v>90</v>
       </c>
@@ -1770,7 +1782,7 @@
       <c r="D81" s="27"/>
       <c r="E81" s="4"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="24" t="s">
         <v>0</v>
       </c>
@@ -1785,7 +1797,7 @@
       </c>
       <c r="E82" s="4"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="20" t="s">
         <v>13</v>
       </c>
@@ -1797,7 +1809,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="20" t="s">
         <v>71</v>
       </c>
@@ -1811,7 +1823,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="20" t="s">
         <v>68</v>
       </c>
@@ -1825,7 +1837,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="20" t="s">
         <v>74</v>
       </c>
@@ -1837,7 +1849,7 @@
       </c>
       <c r="D86" s="20"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="20" t="s">
         <v>20</v>
       </c>
@@ -1847,7 +1859,7 @@
       <c r="C87" s="20"/>
       <c r="D87" s="20"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="20" t="s">
         <v>60</v>
       </c>
@@ -1861,7 +1873,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="20" t="s">
         <v>17</v>
       </c>
@@ -1871,7 +1883,7 @@
       <c r="C89" s="20"/>
       <c r="D89" s="20"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="20" t="s">
         <v>14</v>
       </c>
@@ -1881,16 +1893,16 @@
       <c r="C90" s="20"/>
       <c r="D90" s="20"/>
     </row>
-    <row r="91" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="92" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A92" s="28" t="s">
+    <row r="91" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="92" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A92" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="B92" s="28"/>
-      <c r="C92" s="28"/>
-      <c r="D92" s="28"/>
-    </row>
-    <row r="93" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B92" s="29"/>
+      <c r="C92" s="29"/>
+      <c r="D92" s="29"/>
+    </row>
+    <row r="93" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="26" t="s">
         <v>98</v>
       </c>
@@ -1898,7 +1910,7 @@
       <c r="C93" s="27"/>
       <c r="D93" s="27"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="24" t="s">
         <v>0</v>
       </c>
@@ -1912,7 +1924,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="20" t="s">
         <v>42</v>
       </c>
@@ -1926,7 +1938,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="20" t="s">
         <v>28</v>
       </c>
@@ -1940,7 +1952,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="20" t="s">
         <v>10</v>
       </c>
@@ -1950,32 +1962,32 @@
       <c r="C97" s="20"/>
       <c r="D97" s="20"/>
     </row>
-    <row r="98" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="99" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A99" s="28" t="s">
+    <row r="98" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="99" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A99" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="B99" s="28"/>
-      <c r="C99" s="28"/>
-      <c r="D99" s="28"/>
-    </row>
-    <row r="100" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A100" s="29" t="s">
+      <c r="B99" s="29"/>
+      <c r="C99" s="29"/>
+      <c r="D99" s="29"/>
+    </row>
+    <row r="100" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="B100" s="30"/>
-      <c r="C100" s="30"/>
-      <c r="D100" s="30"/>
-    </row>
-    <row r="101" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="B101" s="31"/>
-      <c r="C101" s="31"/>
-      <c r="D101" s="31"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B100" s="33"/>
+      <c r="C100" s="33"/>
+      <c r="D100" s="33"/>
+    </row>
+    <row r="101" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B101" s="34"/>
+      <c r="C101" s="34"/>
+      <c r="D101" s="34"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="24" t="s">
         <v>0</v>
       </c>
@@ -1990,7 +2002,7 @@
       </c>
       <c r="E102" s="4"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="20" t="s">
         <v>5</v>
       </c>
@@ -2004,7 +2016,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="20" t="s">
         <v>102</v>
       </c>
@@ -2019,19 +2031,19 @@
       </c>
       <c r="E104" s="4"/>
     </row>
-    <row r="105" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E105" s="4"/>
     </row>
-    <row r="106" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A106" s="28" t="s">
+    <row r="106" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A106" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="B106" s="28"/>
-      <c r="C106" s="28"/>
-      <c r="D106" s="28"/>
+      <c r="B106" s="29"/>
+      <c r="C106" s="29"/>
+      <c r="D106" s="29"/>
       <c r="E106" s="4"/>
     </row>
-    <row r="107" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="26" t="s">
         <v>101</v>
       </c>
@@ -2040,7 +2052,7 @@
       <c r="D107" s="27"/>
       <c r="E107" s="4"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="24" t="s">
         <v>0</v>
       </c>
@@ -2055,7 +2067,7 @@
       </c>
       <c r="E108" s="4"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="20" t="s">
         <v>9</v>
       </c>
@@ -2068,126 +2080,151 @@
       <c r="D109" s="20"/>
       <c r="E109" s="4"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="20" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B110" s="21">
         <v>8</v>
       </c>
-      <c r="C110" s="20"/>
+      <c r="C110" s="19" t="s">
+        <v>110</v>
+      </c>
       <c r="D110" s="20"/>
       <c r="E110" s="4"/>
     </row>
-    <row r="111" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B111" s="21">
+        <v>8</v>
+      </c>
+      <c r="C111" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D111" s="20"/>
       <c r="E111" s="4"/>
     </row>
-    <row r="112" spans="1:5" ht="21" x14ac:dyDescent="0.65">
-      <c r="A112" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="B112" s="28"/>
-      <c r="C112" s="28"/>
-      <c r="D112" s="28"/>
+    <row r="112" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E112" s="4"/>
     </row>
-    <row r="113" spans="1:5" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A113" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="B113" s="27"/>
-      <c r="C113" s="27"/>
-      <c r="D113" s="27"/>
+    <row r="113" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A113" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B113" s="29"/>
+      <c r="C113" s="29"/>
+      <c r="D113" s="29"/>
       <c r="E113" s="4"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A114" s="24" t="s">
+    <row r="114" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="B114" s="27"/>
+      <c r="C114" s="27"/>
+      <c r="D114" s="27"/>
+      <c r="E114" s="4"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B114" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C114" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D114" s="24" t="s">
+      <c r="B115" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C115" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D115" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="E114" s="4"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A115" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B115" s="21">
-        <v>1</v>
-      </c>
-      <c r="C115" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D115" s="20" t="s">
-        <v>52</v>
-      </c>
       <c r="E115" s="4"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="20" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="B116" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C116" s="20" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="D116" s="20" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E116" s="4"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="20" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="B117" s="21">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C117" s="20"/>
       <c r="D117" s="20"/>
       <c r="E117" s="4"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B118" s="21">
+        <v>15</v>
+      </c>
+      <c r="C118" s="20"/>
+      <c r="D118" s="20"/>
       <c r="E118" s="4"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E119" s="4"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A120" s="2"/>
-      <c r="B120" s="3"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="2"/>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E120" s="4"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="3"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
       <c r="E121" s="4"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A122" s="5"/>
-      <c r="B122" s="6"/>
-      <c r="C122" s="5"/>
-      <c r="D122" s="5"/>
-      <c r="E122" s="5"/>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="2"/>
+      <c r="B122" s="3"/>
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
+      <c r="E122" s="4"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="5"/>
+      <c r="B123" s="6"/>
+      <c r="C123" s="5"/>
+      <c r="D123" s="5"/>
+      <c r="E123" s="5"/>
     </row>
   </sheetData>
   <sortState ref="A96:C97">
     <sortCondition ref="A95"/>
   </sortState>
   <mergeCells count="27">
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A113:D113"/>
+    <mergeCell ref="A114:D114"/>
+    <mergeCell ref="A100:D100"/>
+    <mergeCell ref="A92:D92"/>
+    <mergeCell ref="A93:D93"/>
+    <mergeCell ref="A99:D99"/>
+    <mergeCell ref="A101:D101"/>
+    <mergeCell ref="A106:D106"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A33:D33"/>
     <mergeCell ref="A81:D81"/>
     <mergeCell ref="A40:D40"/>
     <mergeCell ref="A41:D41"/>
@@ -2201,20 +2238,6 @@
     <mergeCell ref="A74:D74"/>
     <mergeCell ref="A75:D75"/>
     <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A112:D112"/>
-    <mergeCell ref="A113:D113"/>
-    <mergeCell ref="A100:D100"/>
-    <mergeCell ref="A92:D92"/>
-    <mergeCell ref="A93:D93"/>
-    <mergeCell ref="A99:D99"/>
-    <mergeCell ref="A101:D101"/>
-    <mergeCell ref="A106:D106"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
@@ -2229,7 +2252,7 @@
     <hyperlink ref="A93" r:id="rId10"/>
     <hyperlink ref="A100" r:id="rId11"/>
     <hyperlink ref="A107" r:id="rId12"/>
-    <hyperlink ref="A113" r:id="rId13"/>
+    <hyperlink ref="A114" r:id="rId13" display="https://www.youtube.com/watch?v=tNwU7pK_3tk"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="86" fitToHeight="0" orientation="landscape" r:id="rId14"/>

</xml_diff>

<commit_message>
Fixed incorrect part name
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="118">
   <si>
     <t>Part</t>
   </si>
@@ -375,6 +375,15 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=dHWFpkGsxOs</t>
+  </si>
+  <si>
+    <t>74LS138</t>
+  </si>
+  <si>
+    <t>Dual 3-to-8 line decoder</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/sn54ls138.pdf</t>
   </si>
 </sst>
 </file>
@@ -554,13 +563,22 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -570,15 +588,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -867,8 +876,8 @@
   </sheetPr>
   <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,20 +890,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
@@ -964,21 +973,21 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1152,20 +1161,20 @@
       <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
     </row>
     <row r="27" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
@@ -1228,21 +1237,21 @@
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1309,21 +1318,21 @@
       <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
       <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
       <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1401,21 +1410,21 @@
       <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="23" t="s">
+      <c r="A49" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
       <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1490,21 +1499,21 @@
       <c r="E55" s="2"/>
     </row>
     <row r="56" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="B56" s="25"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
       <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="23" t="s">
+      <c r="A57" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="B57" s="24"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="25"/>
       <c r="E57" s="2"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1696,21 +1705,21 @@
       <c r="E73" s="2"/>
     </row>
     <row r="74" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A74" s="25" t="s">
+      <c r="A74" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="B74" s="25"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
+      <c r="B74" s="23"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="23"/>
       <c r="E74" s="2"/>
     </row>
     <row r="75" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="23" t="s">
+      <c r="A75" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="B75" s="24"/>
-      <c r="C75" s="24"/>
-      <c r="D75" s="24"/>
+      <c r="B75" s="25"/>
+      <c r="C75" s="25"/>
+      <c r="D75" s="25"/>
       <c r="E75" s="2"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -1764,21 +1773,21 @@
       <c r="E79" s="2"/>
     </row>
     <row r="80" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A80" s="25" t="s">
+      <c r="A80" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="B80" s="25"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
+      <c r="B80" s="23"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="23"/>
       <c r="E80" s="2"/>
     </row>
     <row r="81" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="23" t="s">
+      <c r="A81" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="B81" s="24"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
+      <c r="B81" s="25"/>
+      <c r="C81" s="25"/>
+      <c r="D81" s="25"/>
       <c r="E81" s="2"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -1894,20 +1903,20 @@
     </row>
     <row r="91" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="92" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A92" s="25" t="s">
+      <c r="A92" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="B92" s="25"/>
-      <c r="C92" s="25"/>
-      <c r="D92" s="25"/>
+      <c r="B92" s="23"/>
+      <c r="C92" s="23"/>
+      <c r="D92" s="23"/>
     </row>
     <row r="93" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="23" t="s">
+      <c r="A93" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="B93" s="24"/>
-      <c r="C93" s="24"/>
-      <c r="D93" s="24"/>
+      <c r="B93" s="25"/>
+      <c r="C93" s="25"/>
+      <c r="D93" s="25"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="21" t="s">
@@ -1963,28 +1972,28 @@
     </row>
     <row r="98" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="99" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A99" s="25" t="s">
+      <c r="A99" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="B99" s="25"/>
-      <c r="C99" s="25"/>
-      <c r="D99" s="25"/>
+      <c r="B99" s="23"/>
+      <c r="C99" s="23"/>
+      <c r="D99" s="23"/>
     </row>
     <row r="100" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="26" t="s">
+      <c r="A100" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="B100" s="27"/>
-      <c r="C100" s="27"/>
-      <c r="D100" s="27"/>
+      <c r="B100" s="30"/>
+      <c r="C100" s="30"/>
+      <c r="D100" s="30"/>
     </row>
     <row r="101" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="28" t="s">
+      <c r="A101" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="B101" s="28"/>
-      <c r="C101" s="28"/>
-      <c r="D101" s="28"/>
+      <c r="B101" s="31"/>
+      <c r="C101" s="31"/>
+      <c r="D101" s="31"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="21" t="s">
@@ -2034,21 +2043,21 @@
       <c r="E105" s="2"/>
     </row>
     <row r="106" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A106" s="25" t="s">
+      <c r="A106" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="B106" s="25"/>
-      <c r="C106" s="25"/>
-      <c r="D106" s="25"/>
+      <c r="B106" s="23"/>
+      <c r="C106" s="23"/>
+      <c r="D106" s="23"/>
       <c r="E106" s="2"/>
     </row>
     <row r="107" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="23" t="s">
+      <c r="A107" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="B107" s="24"/>
-      <c r="C107" s="24"/>
-      <c r="D107" s="24"/>
+      <c r="B107" s="25"/>
+      <c r="C107" s="25"/>
+      <c r="D107" s="25"/>
       <c r="E107" s="2"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2109,21 +2118,21 @@
       <c r="E112" s="2"/>
     </row>
     <row r="113" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A113" s="25" t="s">
+      <c r="A113" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="B113" s="25"/>
-      <c r="C113" s="25"/>
-      <c r="D113" s="25"/>
+      <c r="B113" s="23"/>
+      <c r="C113" s="23"/>
+      <c r="D113" s="23"/>
       <c r="E113" s="2"/>
     </row>
     <row r="114" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="23" t="s">
+      <c r="A114" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="B114" s="24"/>
-      <c r="C114" s="24"/>
-      <c r="D114" s="24"/>
+      <c r="B114" s="25"/>
+      <c r="C114" s="25"/>
+      <c r="D114" s="25"/>
       <c r="E114" s="2"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -2182,21 +2191,21 @@
       <c r="E119" s="2"/>
     </row>
     <row r="120" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A120" s="25" t="s">
+      <c r="A120" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B120" s="25"/>
-      <c r="C120" s="25"/>
-      <c r="D120" s="25"/>
+      <c r="B120" s="23"/>
+      <c r="C120" s="23"/>
+      <c r="D120" s="23"/>
       <c r="E120" s="2"/>
     </row>
     <row r="121" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="23" t="s">
+      <c r="A121" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="B121" s="24"/>
-      <c r="C121" s="24"/>
-      <c r="D121" s="24"/>
+      <c r="B121" s="25"/>
+      <c r="C121" s="25"/>
+      <c r="D121" s="25"/>
       <c r="E121" s="2"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
@@ -2245,16 +2254,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="17" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="B125" s="18">
         <v>1</v>
       </c>
       <c r="C125" s="17" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="D125" s="17" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -2292,35 +2301,35 @@
     <sortCondition ref="A95"/>
   </sortState>
   <mergeCells count="29">
+    <mergeCell ref="A99:D99"/>
+    <mergeCell ref="A101:D101"/>
+    <mergeCell ref="A106:D106"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A34:D34"/>
     <mergeCell ref="A120:D120"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A81:D81"/>
     <mergeCell ref="A40:D40"/>
     <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A34:D34"/>
     <mergeCell ref="A56:D56"/>
     <mergeCell ref="A57:D57"/>
     <mergeCell ref="A74:D74"/>
     <mergeCell ref="A75:D75"/>
     <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A33:D33"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A113:D113"/>
     <mergeCell ref="A114:D114"/>
     <mergeCell ref="A100:D100"/>
     <mergeCell ref="A92:D92"/>
     <mergeCell ref="A93:D93"/>
-    <mergeCell ref="A99:D99"/>
-    <mergeCell ref="A101:D101"/>
-    <mergeCell ref="A106:D106"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed broken link to datasheet
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14388"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18372" windowHeight="6588"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="2" r:id="rId1"/>
+    <sheet name="_ignore" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Modules!$A$29:$D$31</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="127">
   <si>
     <t>Part</t>
   </si>
@@ -191,9 +192,6 @@
     <t>http://www.ti.com/lit/ds/symlink/sn74ls161a.pdf</t>
   </si>
   <si>
-    <t>http://www.ti.com/lit/ds/symlink/sn74173.pdf</t>
-  </si>
-  <si>
     <t>http://www.ndatasheet.com/datasheet-frame/300/mdownload.php?id=529296</t>
   </si>
   <si>
@@ -384,6 +382,36 @@
   </si>
   <si>
     <t>http://www.ti.com/lit/ds/symlink/sn54ls138.pdf</t>
+  </si>
+  <si>
+    <t>74F269 (8-bit counter)</t>
+  </si>
+  <si>
+    <t>https://nl.mouser.com/ProductDetail/BusBoard-Prototype-Systems/BB830/?qs=sGAEpiMZZMuwa3xtPTB8C%2f9n%252bwN0SKyc1WVkAjVIZyw=</t>
+  </si>
+  <si>
+    <t>BB830 breadboard</t>
+  </si>
+  <si>
+    <t>http://pdf1.alldatasheet.com/datasheet-pdf/view/133278/TI/SN74LS384N.html</t>
+  </si>
+  <si>
+    <t>SN74LS384 (Multiplier)</t>
+  </si>
+  <si>
+    <t>74181 ALU</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/74181</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/464/IDT_71256SA_DST_2014113-881483.pdf</t>
+  </si>
+  <si>
+    <t>IDT71256SA (256 kbit RAM)</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/sn74ls173a.pdf</t>
   </si>
 </sst>
 </file>
@@ -523,7 +551,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -563,6 +591,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -575,19 +605,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -876,8 +906,8 @@
   </sheetPr>
   <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="D125" sqref="D125"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -890,20 +920,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="A1" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
+      <c r="A2" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
@@ -943,16 +973,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="18">
+        <v>1</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="18">
-        <v>1</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>61</v>
+      <c r="D6" s="24" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -973,21 +1003,21 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A9" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
+      <c r="A9" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+      <c r="A10" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1012,7 +1042,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="16"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="24" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1026,7 +1056,7 @@
       <c r="C13" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="24" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1040,7 +1070,7 @@
       <c r="C14" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="24" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1054,8 +1084,8 @@
       <c r="C15" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>57</v>
+      <c r="D15" s="24" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1144,13 +1174,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" s="18">
         <v>1</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D24" s="16"/>
     </row>
@@ -1161,20 +1191,20 @@
       <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
+      <c r="A26" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
     </row>
     <row r="27" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
+      <c r="A27" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
@@ -1201,8 +1231,8 @@
       <c r="C29" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="17" t="s">
-        <v>53</v>
+      <c r="D29" s="24" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1215,8 +1245,8 @@
       <c r="C30" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="17" t="s">
-        <v>55</v>
+      <c r="D30" s="24" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1237,21 +1267,21 @@
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A33" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
+      <c r="A33" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
+      <c r="A34" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1279,8 +1309,8 @@
       <c r="C36" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="17" t="s">
-        <v>53</v>
+      <c r="D36" s="24" t="s">
+        <v>126</v>
       </c>
       <c r="E36" s="2"/>
     </row>
@@ -1294,8 +1324,8 @@
       <c r="C37" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D37" s="17" t="s">
-        <v>55</v>
+      <c r="D37" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="E37" s="2"/>
     </row>
@@ -1318,21 +1348,21 @@
       <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A40" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
+      <c r="A40" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
       <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="A41" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
       <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1360,8 +1390,8 @@
       <c r="C43" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D43" s="17" t="s">
-        <v>53</v>
+      <c r="D43" s="24" t="s">
+        <v>126</v>
       </c>
       <c r="E43" s="2"/>
     </row>
@@ -1375,8 +1405,8 @@
       <c r="C44" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D44" s="17" t="s">
-        <v>55</v>
+      <c r="D44" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="E44" s="2"/>
     </row>
@@ -1410,21 +1440,21 @@
       <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
+      <c r="A49" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
       <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1452,8 +1482,8 @@
       <c r="C51" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D51" s="17" t="s">
-        <v>55</v>
+      <c r="D51" s="24" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -1466,8 +1496,8 @@
       <c r="C52" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D52" s="17" t="s">
-        <v>56</v>
+      <c r="D52" s="24" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -1480,8 +1510,8 @@
       <c r="C53" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="17" t="s">
-        <v>58</v>
+      <c r="D53" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1499,21 +1529,21 @@
       <c r="E55" s="2"/>
     </row>
     <row r="56" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A56" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
+      <c r="A56" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="25"/>
+      <c r="C56" s="25"/>
+      <c r="D56" s="25"/>
       <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="B57" s="25"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
+      <c r="A57" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" s="27"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
       <c r="E57" s="2"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1541,7 +1571,7 @@
       <c r="C59" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D59" s="24" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1555,7 +1585,7 @@
       <c r="C60" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D60" s="17" t="s">
+      <c r="D60" s="24" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1569,7 +1599,7 @@
       <c r="C61" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D61" s="17" t="s">
+      <c r="D61" s="24" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1583,8 +1613,8 @@
       <c r="C62" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D62" s="17" t="s">
-        <v>53</v>
+      <c r="D62" s="24" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1597,8 +1627,8 @@
       <c r="C63" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D63" s="17" t="s">
-        <v>54</v>
+      <c r="D63" s="24" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -1611,13 +1641,13 @@
       <c r="C64" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D64" s="17" t="s">
-        <v>55</v>
+      <c r="D64" s="24" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B65" s="18">
         <v>1</v>
@@ -1627,7 +1657,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B66" s="18">
         <v>1</v>
@@ -1705,21 +1735,21 @@
       <c r="E73" s="2"/>
     </row>
     <row r="74" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A74" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="B74" s="23"/>
-      <c r="C74" s="23"/>
-      <c r="D74" s="23"/>
+      <c r="A74" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B74" s="25"/>
+      <c r="C74" s="25"/>
+      <c r="D74" s="25"/>
       <c r="E74" s="2"/>
     </row>
     <row r="75" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="B75" s="25"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="25"/>
+      <c r="A75" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B75" s="27"/>
+      <c r="C75" s="27"/>
+      <c r="D75" s="27"/>
       <c r="E75" s="2"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -1739,30 +1769,30 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B77" s="18">
+        <v>2</v>
+      </c>
+      <c r="C77" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B77" s="18">
-        <v>2</v>
-      </c>
-      <c r="C77" s="17" t="s">
+      <c r="D77" s="24" t="s">
         <v>66</v>
-      </c>
-      <c r="D77" s="17" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B78" s="18">
+        <v>1</v>
+      </c>
+      <c r="C78" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B78" s="18">
-        <v>1</v>
-      </c>
-      <c r="C78" s="17" t="s">
+      <c r="D78" s="24" t="s">
         <v>63</v>
-      </c>
-      <c r="D78" s="17" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1773,21 +1803,21 @@
       <c r="E79" s="2"/>
     </row>
     <row r="80" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A80" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="B80" s="23"/>
-      <c r="C80" s="23"/>
-      <c r="D80" s="23"/>
+      <c r="A80" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B80" s="25"/>
+      <c r="C80" s="25"/>
+      <c r="D80" s="25"/>
       <c r="E80" s="2"/>
     </row>
     <row r="81" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="B81" s="25"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="25"/>
+      <c r="A81" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B81" s="27"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
       <c r="E81" s="2"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -1813,47 +1843,47 @@
         <v>1</v>
       </c>
       <c r="C83" s="17"/>
-      <c r="D83" s="17" t="s">
+      <c r="D83" s="24" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B84" s="18">
+        <v>1</v>
+      </c>
+      <c r="C84" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B84" s="18">
-        <v>1</v>
-      </c>
-      <c r="C84" s="17" t="s">
+      <c r="D84" s="24" t="s">
         <v>72</v>
-      </c>
-      <c r="D84" s="17" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B85" s="18">
+        <v>1</v>
+      </c>
+      <c r="C85" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B85" s="18">
-        <v>1</v>
-      </c>
-      <c r="C85" s="17" t="s">
+      <c r="D85" s="24" t="s">
         <v>69</v>
-      </c>
-      <c r="D85" s="17" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B86" s="18">
         <v>4</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D86" s="17"/>
     </row>
@@ -1869,16 +1899,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B88" s="18">
         <v>1</v>
       </c>
       <c r="C88" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="D88" s="17" t="s">
-        <v>59</v>
+        <v>95</v>
+      </c>
+      <c r="D88" s="24" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -1903,20 +1933,20 @@
     </row>
     <row r="91" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="92" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A92" s="23" t="s">
+      <c r="A92" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92" s="25"/>
+      <c r="C92" s="25"/>
+      <c r="D92" s="25"/>
+    </row>
+    <row r="93" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B92" s="23"/>
-      <c r="C92" s="23"/>
-      <c r="D92" s="23"/>
-    </row>
-    <row r="93" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="B93" s="25"/>
-      <c r="C93" s="25"/>
-      <c r="D93" s="25"/>
+      <c r="B93" s="27"/>
+      <c r="C93" s="27"/>
+      <c r="D93" s="27"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="21" t="s">
@@ -1942,7 +1972,7 @@
       <c r="C95" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D95" s="17" t="s">
+      <c r="D95" s="24" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1956,8 +1986,8 @@
       <c r="C96" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D96" s="17" t="s">
-        <v>55</v>
+      <c r="D96" s="24" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
@@ -1972,28 +2002,28 @@
     </row>
     <row r="98" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="99" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A99" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="B99" s="23"/>
-      <c r="C99" s="23"/>
-      <c r="D99" s="23"/>
+      <c r="A99" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B99" s="25"/>
+      <c r="C99" s="25"/>
+      <c r="D99" s="25"/>
     </row>
     <row r="100" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B100" s="30"/>
       <c r="C100" s="30"/>
       <c r="D100" s="30"/>
     </row>
     <row r="101" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="B101" s="31"/>
-      <c r="C101" s="31"/>
-      <c r="D101" s="31"/>
+      <c r="A101" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B101" s="32"/>
+      <c r="C101" s="32"/>
+      <c r="D101" s="32"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="21" t="s">
@@ -2020,22 +2050,22 @@
       <c r="C103" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D103" s="17" t="s">
+      <c r="D103" s="24" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B104" s="18">
+        <v>1</v>
+      </c>
+      <c r="C104" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="B104" s="18">
-        <v>1</v>
-      </c>
-      <c r="C104" s="17" t="s">
+      <c r="D104" s="24" t="s">
         <v>103</v>
-      </c>
-      <c r="D104" s="17" t="s">
-        <v>104</v>
       </c>
       <c r="E104" s="2"/>
     </row>
@@ -2043,21 +2073,21 @@
       <c r="E105" s="2"/>
     </row>
     <row r="106" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A106" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="B106" s="23"/>
-      <c r="C106" s="23"/>
-      <c r="D106" s="23"/>
+      <c r="A106" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B106" s="25"/>
+      <c r="C106" s="25"/>
+      <c r="D106" s="25"/>
       <c r="E106" s="2"/>
     </row>
     <row r="107" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="B107" s="25"/>
-      <c r="C107" s="25"/>
-      <c r="D107" s="25"/>
+      <c r="A107" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B107" s="27"/>
+      <c r="C107" s="27"/>
+      <c r="D107" s="27"/>
       <c r="E107" s="2"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2083,33 +2113,33 @@
         <v>8</v>
       </c>
       <c r="C109" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D109" s="17"/>
       <c r="E109" s="2"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B110" s="18">
         <v>8</v>
       </c>
       <c r="C110" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D110" s="17"/>
       <c r="E110" s="2"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B111" s="18">
         <v>8</v>
       </c>
       <c r="C111" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D111" s="17"/>
       <c r="E111" s="2"/>
@@ -2118,21 +2148,21 @@
       <c r="E112" s="2"/>
     </row>
     <row r="113" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A113" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="B113" s="23"/>
-      <c r="C113" s="23"/>
-      <c r="D113" s="23"/>
+      <c r="A113" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B113" s="25"/>
+      <c r="C113" s="25"/>
+      <c r="D113" s="25"/>
       <c r="E113" s="2"/>
     </row>
     <row r="114" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="B114" s="25"/>
-      <c r="C114" s="25"/>
-      <c r="D114" s="25"/>
+      <c r="A114" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B114" s="27"/>
+      <c r="C114" s="27"/>
+      <c r="D114" s="27"/>
       <c r="E114" s="2"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -2160,14 +2190,14 @@
       <c r="C116" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D116" s="17" t="s">
+      <c r="D116" s="24" t="s">
         <v>47</v>
       </c>
       <c r="E116" s="2"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B117" s="18">
         <v>15</v>
@@ -2191,21 +2221,21 @@
       <c r="E119" s="2"/>
     </row>
     <row r="120" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A120" s="23" t="s">
+      <c r="A120" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="B120" s="25"/>
+      <c r="C120" s="25"/>
+      <c r="D120" s="25"/>
+      <c r="E120" s="2"/>
+    </row>
+    <row r="121" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="B120" s="23"/>
-      <c r="C120" s="23"/>
-      <c r="D120" s="23"/>
-      <c r="E120" s="2"/>
-    </row>
-    <row r="121" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="B121" s="25"/>
-      <c r="C121" s="25"/>
-      <c r="D121" s="25"/>
+      <c r="B121" s="27"/>
+      <c r="C121" s="27"/>
+      <c r="D121" s="27"/>
       <c r="E121" s="2"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
@@ -2225,16 +2255,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B123" s="18">
         <v>2</v>
       </c>
       <c r="C123" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="D123" s="17" t="s">
-        <v>59</v>
+        <v>95</v>
+      </c>
+      <c r="D123" s="24" t="s">
+        <v>58</v>
       </c>
       <c r="E123" s="3"/>
     </row>
@@ -2248,22 +2278,22 @@
       <c r="C124" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D124" s="17" t="s">
+      <c r="D124" s="24" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B125" s="18">
+        <v>1</v>
+      </c>
+      <c r="C125" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="B125" s="18">
-        <v>1</v>
-      </c>
-      <c r="C125" s="17" t="s">
+      <c r="D125" s="24" t="s">
         <v>116</v>
-      </c>
-      <c r="D125" s="17" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -2307,12 +2337,12 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A49:D49"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A49:D49"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="A120:D120"/>
     <mergeCell ref="A121:D121"/>
@@ -2346,8 +2376,100 @@
     <hyperlink ref="A107" r:id="rId12"/>
     <hyperlink ref="A114" r:id="rId13" display="https://www.youtube.com/watch?v=tNwU7pK_3tk"/>
     <hyperlink ref="A121" r:id="rId14" display="https://www.youtube.com/watch?v=tNwU7pK_3tk"/>
+    <hyperlink ref="D63" r:id="rId15"/>
+    <hyperlink ref="D62" r:id="rId16"/>
+    <hyperlink ref="D6" r:id="rId17"/>
+    <hyperlink ref="D12" r:id="rId18"/>
+    <hyperlink ref="D13" r:id="rId19"/>
+    <hyperlink ref="D14" r:id="rId20"/>
+    <hyperlink ref="D15" r:id="rId21"/>
+    <hyperlink ref="D29" r:id="rId22"/>
+    <hyperlink ref="D30" r:id="rId23"/>
+    <hyperlink ref="D36" r:id="rId24"/>
+    <hyperlink ref="D37" r:id="rId25"/>
+    <hyperlink ref="D43" r:id="rId26"/>
+    <hyperlink ref="D44" r:id="rId27"/>
+    <hyperlink ref="D51" r:id="rId28"/>
+    <hyperlink ref="D52" r:id="rId29"/>
+    <hyperlink ref="D53" r:id="rId30"/>
+    <hyperlink ref="D59" r:id="rId31"/>
+    <hyperlink ref="D60" r:id="rId32"/>
+    <hyperlink ref="D61" r:id="rId33"/>
+    <hyperlink ref="D64" r:id="rId34"/>
+    <hyperlink ref="D77" r:id="rId35"/>
+    <hyperlink ref="D78" r:id="rId36"/>
+    <hyperlink ref="D83" r:id="rId37"/>
+    <hyperlink ref="D84" r:id="rId38"/>
+    <hyperlink ref="D85" r:id="rId39"/>
+    <hyperlink ref="D88" r:id="rId40"/>
+    <hyperlink ref="D95" r:id="rId41"/>
+    <hyperlink ref="D96" r:id="rId42"/>
+    <hyperlink ref="D103" r:id="rId43"/>
+    <hyperlink ref="D104" r:id="rId44"/>
+    <hyperlink ref="D116" r:id="rId45"/>
+    <hyperlink ref="D123" r:id="rId46"/>
+    <hyperlink ref="D124" r:id="rId47"/>
+    <hyperlink ref="D125" r:id="rId48"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="86" fitToHeight="0" orientation="landscape" r:id="rId15"/>
+  <pageSetup paperSize="9" scale="86" fitToHeight="0" orientation="landscape" r:id="rId49"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>